<commit_message>
Increased dataset size and switched to random forest
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -1,35 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarik\OneDrive\Documents\Code\PoseFinder\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6168B5D7-606C-4266-981B-5513DD067EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F33C4AA-0E80-4EC0-BB55-7BECCDA83ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
   <si>
     <t>Initial</t>
   </si>
   <si>
+    <t>DataSet Size</t>
+  </si>
+  <si>
+    <t>Classification Model</t>
+  </si>
+  <si>
     <t>Class</t>
   </si>
   <si>
@@ -45,6 +52,9 @@
     <t>Support</t>
   </si>
   <si>
+    <t>TensorFlow Keras NN</t>
+  </si>
+  <si>
     <t>Accuracy</t>
   </si>
   <si>
@@ -54,16 +64,25 @@
     <t>Weighted Avg</t>
   </si>
   <si>
-    <t>DataSet Size</t>
-  </si>
-  <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>Parameters</t>
-  </si>
-  <si>
     <t>Increased Dataset Size</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>macro avg</t>
+  </si>
+  <si>
+    <t>weighted avg</t>
+  </si>
+  <si>
+    <t>Changed Classification Model</t>
+  </si>
+  <si>
+    <t>RandomForest</t>
   </si>
 </sst>
 </file>
@@ -95,7 +114,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,6 +139,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -133,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -141,26 +172,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,70 +490,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.21875" customWidth="1"/>
-    <col min="7" max="7" width="15" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15" style="3" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="3">
+        <v>30</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="4">
-        <v>30</v>
-      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="17">
         <v>0</v>
       </c>
       <c r="B4" s="2">
@@ -521,7 +577,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="17">
         <v>1</v>
       </c>
       <c r="B5" s="2">
@@ -538,8 +594,8 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
+      <c r="A6" s="16" t="s">
+        <v>11</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -551,8 +607,8 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
+      <c r="A7" s="16" t="s">
+        <v>12</v>
       </c>
       <c r="B7" s="2">
         <v>0.33</v>
@@ -568,8 +624,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
+      <c r="A8" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="B8" s="2">
         <v>0.44</v>
@@ -585,43 +641,46 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="A11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>1</v>
+      <c r="A12" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="4">
+        <v>9</v>
+      </c>
+      <c r="G12" s="3">
         <v>60</v>
       </c>
+      <c r="H12" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="17">
         <v>0</v>
       </c>
       <c r="B13" s="2">
@@ -638,7 +697,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14" s="17">
         <v>1</v>
       </c>
       <c r="B14" s="2">
@@ -655,8 +714,8 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>6</v>
+      <c r="A15" s="16" t="s">
+        <v>11</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -668,8 +727,8 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
+      <c r="A16" s="16" t="s">
+        <v>12</v>
       </c>
       <c r="B16" s="2">
         <v>0.83</v>
@@ -684,9 +743,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>8</v>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="B17" s="2">
         <v>0.89</v>
@@ -701,14 +760,232 @@
         <v>12</v>
       </c>
     </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="3">
+        <v>100</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D21">
+        <v>0.73684210526315785</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22">
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0.78260869565217395</v>
+      </c>
+      <c r="E22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23">
+        <v>0.8214285714285714</v>
+      </c>
+      <c r="C23">
+        <v>0.79166666666666674</v>
+      </c>
+      <c r="D23">
+        <v>0.7597254004576659</v>
+      </c>
+      <c r="E23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24">
+        <v>0.84693877551020402</v>
+      </c>
+      <c r="C24">
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="D24">
+        <v>0.75645635828702196</v>
+      </c>
+      <c r="E24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>0.76190476190476186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="3">
+        <v>100</v>
+      </c>
+      <c r="H28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D29">
+        <v>0.95652173913043481</v>
+      </c>
+      <c r="E29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <v>0.9</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0.94736842105263153</v>
+      </c>
+      <c r="E30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31">
+        <v>0.95</v>
+      </c>
+      <c r="C31">
+        <v>0.95833333333333326</v>
+      </c>
+      <c r="D31">
+        <v>0.95194508009153322</v>
+      </c>
+      <c r="E31">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>0.95714285714285718</v>
+      </c>
+      <c r="C32">
+        <v>0.95238095238095233</v>
+      </c>
+      <c r="D32">
+        <v>0.9525988885256621</v>
+      </c>
+      <c r="E32">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33">
+        <v>0.95238095238095233</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="A27:E27"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A11:E11"/>
     <mergeCell ref="G1:J1"/>
-    <mergeCell ref="A11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>